<commit_message>
Last commit before real pilot test.
</commit_message>
<xml_diff>
--- a/PathPlanner/UserStudyData/Groups.xlsx
+++ b/PathPlanner/UserStudyData/Groups.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="18870" windowHeight="11250"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Group ID</t>
   </si>
@@ -44,12 +44,33 @@
   <si>
     <t>Slide With Diff</t>
   </si>
+  <si>
+    <t>Pilot Study</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>User Study</t>
+  </si>
+  <si>
+    <t>First Scenario</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -80,20 +101,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -172,6 +287,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -206,6 +322,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,30 +498,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(1, 6)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -427,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -450,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -473,7 +593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -496,7 +616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -519,7 +639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -542,16 +662,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="I9">
         <f ca="1">RANDBETWEEN(7, 12)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -574,7 +694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -597,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -620,7 +740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -643,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -666,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -689,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -697,7 +817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -705,7 +825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -713,7 +833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -721,7 +841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>5</v>
       </c>
@@ -729,13 +849,511 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <f ca="1">RANDBETWEEN(1,6)</f>
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <f ca="1">RANDBETWEEN(7,12)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>1</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>2</v>
+      </c>
+      <c r="B39" s="7">
+        <v>2</v>
+      </c>
+      <c r="C39" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>3</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>4</v>
+      </c>
+      <c r="B41" s="7">
+        <v>2</v>
+      </c>
+      <c r="C41" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>5</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>6</v>
+      </c>
+      <c r="B43" s="7">
+        <v>2</v>
+      </c>
+      <c r="C43" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>7</v>
+      </c>
+      <c r="B44" s="7">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>8</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2</v>
+      </c>
+      <c r="C45" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>9</v>
+      </c>
+      <c r="B46" s="7">
+        <v>1</v>
+      </c>
+      <c r="C46" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>10</v>
+      </c>
+      <c r="B47" s="7">
+        <v>2</v>
+      </c>
+      <c r="C47" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>11</v>
+      </c>
+      <c r="B48" s="7">
+        <v>1</v>
+      </c>
+      <c r="C48" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>12</v>
+      </c>
+      <c r="B49" s="10">
+        <v>2</v>
+      </c>
+      <c r="C49" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>13</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>14</v>
+      </c>
+      <c r="B51" s="7">
+        <v>2</v>
+      </c>
+      <c r="C51" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>15</v>
+      </c>
+      <c r="B52" s="7">
+        <v>1</v>
+      </c>
+      <c r="C52" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>16</v>
+      </c>
+      <c r="B53" s="7">
+        <v>2</v>
+      </c>
+      <c r="C53" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>17</v>
+      </c>
+      <c r="B54" s="7">
+        <v>1</v>
+      </c>
+      <c r="C54" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>18</v>
+      </c>
+      <c r="B55" s="7">
+        <v>2</v>
+      </c>
+      <c r="C55" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>19</v>
+      </c>
+      <c r="B56" s="7">
+        <v>1</v>
+      </c>
+      <c r="C56" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>20</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2</v>
+      </c>
+      <c r="C57" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>21</v>
+      </c>
+      <c r="B58" s="7">
+        <v>1</v>
+      </c>
+      <c r="C58" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>22</v>
+      </c>
+      <c r="B59" s="7">
+        <v>2</v>
+      </c>
+      <c r="C59" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>23</v>
+      </c>
+      <c r="B60" s="7">
+        <v>1</v>
+      </c>
+      <c r="C60" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>24</v>
+      </c>
+      <c r="B61" s="10">
+        <v>2</v>
+      </c>
+      <c r="C61" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>25</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>26</v>
+      </c>
+      <c r="B63" s="7">
+        <v>2</v>
+      </c>
+      <c r="C63" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>27</v>
+      </c>
+      <c r="B64" s="7">
+        <v>1</v>
+      </c>
+      <c r="C64" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>28</v>
+      </c>
+      <c r="B65" s="7">
+        <v>2</v>
+      </c>
+      <c r="C65" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>29</v>
+      </c>
+      <c r="B66" s="7">
+        <v>1</v>
+      </c>
+      <c r="C66" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>30</v>
+      </c>
+      <c r="B67" s="7">
+        <v>2</v>
+      </c>
+      <c r="C67" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>31</v>
+      </c>
+      <c r="B68" s="7">
+        <v>1</v>
+      </c>
+      <c r="C68" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>32</v>
+      </c>
+      <c r="B69" s="7">
+        <v>2</v>
+      </c>
+      <c r="C69" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -743,16 +1361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -772,7 +1390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -792,7 +1410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -812,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -832,7 +1450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -852,7 +1470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -878,12 +1496,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Still working on slider resolution bug.
</commit_message>
<xml_diff>
--- a/PathPlanner/UserStudyData/Groups.xlsx
+++ b/PathPlanner/UserStudyData/Groups.xlsx
@@ -502,7 +502,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="I9">
         <f ca="1">RANDBETWEEN(7, 12)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -863,11 +863,11 @@
       </c>
       <c r="B26">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <f ca="1">RANDBETWEEN(7,12)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>3</v>
       </c>
     </row>
@@ -908,7 +908,7 @@
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>12</v>
       </c>
     </row>
@@ -919,7 +919,7 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed pattern double click bug
</commit_message>
<xml_diff>
--- a/PathPlanner/UserStudyData/Groups.xlsx
+++ b/PathPlanner/UserStudyData/Groups.xlsx
@@ -726,7 +726,7 @@
       </c>
       <c r="I9">
         <f ca="1">RANDBETWEEN(7, 12)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
       </c>
       <c r="B26">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <f ca="1">RANDBETWEEN(7,12)</f>
@@ -3175,10 +3175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4591,15 +4591,15 @@
       </c>
       <c r="F64">
         <f ca="1">RANDBETWEEN(1,60)</f>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G64">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H64">
         <f ca="1">RANDBETWEEN(31,60)</f>
-        <v>57</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4792,6 +4792,46 @@
       </c>
       <c r="B88">
         <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="13">
+        <v>26</v>
+      </c>
+      <c r="B89">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="13">
+        <v>27</v>
+      </c>
+      <c r="B90">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="13">
+        <v>28</v>
+      </c>
+      <c r="B91">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="13">
+        <v>29</v>
+      </c>
+      <c r="B92">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="13">
+        <v>30</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15 modes for TopN now.
</commit_message>
<xml_diff>
--- a/PathPlanner/UserStudyData/Groups.xlsx
+++ b/PathPlanner/UserStudyData/Groups.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Group ID</t>
   </si>
@@ -185,6 +185,27 @@
   </si>
   <si>
     <t>Lehla Kisor</t>
+  </si>
+  <si>
+    <t>Scott Kim</t>
+  </si>
+  <si>
+    <t>Dallan Carter</t>
+  </si>
+  <si>
+    <t>Mark Murdock</t>
+  </si>
+  <si>
+    <t>Emilae Belo</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Yoomi Kim</t>
   </si>
 </sst>
 </file>
@@ -660,7 +681,7 @@
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(1, 6)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,7 +828,7 @@
       </c>
       <c r="I9">
         <f ca="1">RANDBETWEEN(7, 12)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1002,7 +1023,7 @@
       </c>
       <c r="B26">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <f ca="1">RANDBETWEEN(7,12)</f>
@@ -3256,10 +3277,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4684,15 +4705,15 @@
       </c>
       <c r="F64">
         <f ca="1">RANDBETWEEN(1,60)</f>
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="G64">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H64">
         <f ca="1">RANDBETWEEN(31,60)</f>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -5002,6 +5023,12 @@
       <c r="B86">
         <v>31</v>
       </c>
+      <c r="C86" t="s">
+        <v>59</v>
+      </c>
+      <c r="D86" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="13">
@@ -5010,6 +5037,12 @@
       <c r="B87">
         <v>14</v>
       </c>
+      <c r="C87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D87" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="13">
@@ -5018,6 +5051,12 @@
       <c r="B88">
         <v>55</v>
       </c>
+      <c r="C88" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="13">
@@ -5026,6 +5065,12 @@
       <c r="B89">
         <v>22</v>
       </c>
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="13">
@@ -5034,6 +5079,12 @@
       <c r="B90">
         <v>58</v>
       </c>
+      <c r="C90" t="s">
+        <v>62</v>
+      </c>
+      <c r="D90" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="13">
@@ -5057,6 +5108,24 @@
       </c>
       <c r="B93">
         <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94">
+        <f>COUNTIF(D64:D93, "F")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>61</v>
+      </c>
+      <c r="D95">
+        <f>COUNTIF(D64:D93, "M")</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>